<commit_message>
ajout de divers modification
</commit_message>
<xml_diff>
--- a/Modèle-audit.xlsx
+++ b/Modèle-audit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="624" windowWidth="23256" windowHeight="13176" tabRatio="500"/>
+    <workbookView xWindow="930" yWindow="630" windowWidth="23250" windowHeight="13170" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
   <si>
     <t>Catégorie</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>https://validator.w3.org/</t>
-  </si>
-  <si>
-    <t>Mq balise sementique footer et header</t>
   </si>
   <si>
     <t>Des balise div on etais utiliser à la place des balises sementiques</t>
@@ -385,6 +382,12 @@
   </si>
   <si>
     <t>best practices/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mq balise sementique footer et header section main </t>
+  </si>
+  <si>
+    <t>suppression de li non utiliser</t>
   </si>
 </sst>
 </file>
@@ -837,20 +840,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="21.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.90625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="61.6328125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="10.54296875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="61.6328125" style="9" customWidth="1"/>
-    <col min="10" max="26" width="10.54296875" customWidth="1"/>
+    <col min="1" max="2" width="21.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="61.6640625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="61.6640625" style="9" customWidth="1"/>
+    <col min="10" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -962,7 +965,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>17</v>
@@ -984,7 +987,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>22</v>
@@ -1015,7 +1018,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>24</v>
@@ -1025,53 +1028,53 @@
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:26" s="8" customFormat="1" ht="179.4" customHeight="1">
+    <row r="9" spans="1:26" s="8" customFormat="1" ht="179.45" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="F9" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1082,19 +1085,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1105,16 +1108,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1123,19 +1126,19 @@
     </row>
     <row r="12" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1147,16 +1150,16 @@
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1165,19 +1168,19 @@
     </row>
     <row r="14" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1186,19 +1189,19 @@
     </row>
     <row r="15" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1207,18 +1210,18 @@
     </row>
     <row r="16" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1229,16 +1232,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1250,16 +1253,16 @@
         <v>7</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1271,16 +1274,16 @@
         <v>7</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1289,22 +1292,22 @@
     </row>
     <row r="20" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="F20" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1312,19 +1315,19 @@
     </row>
     <row r="21" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1333,22 +1336,22 @@
     </row>
     <row r="22" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1356,19 +1359,19 @@
     </row>
     <row r="23" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1377,7 +1380,9 @@
     </row>
     <row r="24" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>

</xml_diff>

<commit_message>
modif du fichier xlsx
</commit_message>
<xml_diff>
--- a/Modèle-audit.xlsx
+++ b/Modèle-audit.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="119">
   <si>
     <t>Catégorie</t>
   </si>
@@ -54,9 +54,6 @@
     <t>SEO</t>
   </si>
   <si>
-    <t>lg2</t>
-  </si>
-  <si>
     <t>lang="Default"</t>
   </si>
   <si>
@@ -87,15 +84,9 @@
     <t>&lt;title&gt;.&lt;/title&gt;</t>
   </si>
   <si>
-    <t>lg16 à 20</t>
-  </si>
-  <si>
     <t>https://smartkeyword.io/seo-on-page-balise-title/#:~:text=de%20l'onglet.-,Pourquoi%20la%20balise%20Title%20est%20importante%20en%20SEO%20%3F,et%20positionner%20la%20page%20web.</t>
   </si>
   <si>
-    <t>lg 22</t>
-  </si>
-  <si>
     <t xml:space="preserve">remplacer le , par </t>
   </si>
   <si>
@@ -108,9 +99,6 @@
     <t>meta name="keywords"</t>
   </si>
   <si>
-    <t>lg5</t>
-  </si>
-  <si>
     <t xml:space="preserve">ne pas en utiliser car la balise  est morte voir l'article sur la mort d'une balise </t>
   </si>
   <si>
@@ -288,9 +276,6 @@
     <t>input et texte area ne sont pas dans notre label</t>
   </si>
   <si>
-    <t>wrapper inut et le texte area dans le label</t>
-  </si>
-  <si>
     <t>ou attribuer l'attribue for a mon input et a mon texte area</t>
   </si>
   <si>
@@ -309,9 +294,6 @@
     <t xml:space="preserve">convertire les image au format  WebP ou AVIF </t>
   </si>
   <si>
-    <t>https://web.dev/uses-webp-images/?utm_source=lighthouse&amp;utm_medium=lr</t>
-  </si>
-  <si>
     <t>https://web.dev/color-contrast/?utm_source=lighthouse&amp;utm_medium=lr</t>
   </si>
   <si>
@@ -328,12 +310,6 @@
   </si>
   <si>
     <t>toujour remplir la balise alt avec des mots qui decrive l'image</t>
-  </si>
-  <si>
-    <t>remplire la balise alt dde fasson pertinente</t>
-  </si>
-  <si>
-    <t>https://drafts.csswg.org/mediaqueries/#mf-deprecated</t>
   </si>
   <si>
     <t>device-width</t>
@@ -387,7 +363,50 @@
     <t xml:space="preserve">Mq balise sementique footer et header section main </t>
   </si>
   <si>
-    <t>suppression de li non utiliser</t>
+    <t>https://geekflare.com/fr/remove-seo-spam/</t>
+  </si>
+  <si>
+    <t>bon sens</t>
+  </si>
+  <si>
+    <t>https://web.dev/font-size/?utm_source=lighthouse&amp;utm_medium=lr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://geekflare.com/fr/remove-seo-spam/ </t>
+  </si>
+  <si>
+    <t>Un contraste dont le ratio est de 4.5:1 pour les textes normaux
+Un contraste dont le ratio est de 3:1 pour les grands textes,</t>
+  </si>
+  <si>
+    <t>toujour verifier le ratio entre le background et les font</t>
+  </si>
+  <si>
+    <t>wrapper input et le texte area dans le label</t>
+  </si>
+  <si>
+    <t>suppression des li non utiliser</t>
+  </si>
+  <si>
+    <t>cree les element que au moment du besoin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise li vide dans le code </t>
+  </si>
+  <si>
+    <t>balise li non utile</t>
+  </si>
+  <si>
+    <t>remplire la balise alt de fasson pertinente</t>
+  </si>
+  <si>
+    <t>https://web.dev/label/?utm_source=lighthouse&amp;utm_medium=lr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.dev/uses-webp-images/?utm_source=lighthouse&amp;utm_medium=lr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drafts.csswg.org/mediaqueries/#mf-deprecated </t>
   </si>
 </sst>
 </file>
@@ -469,7 +488,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,12 +499,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -512,7 +525,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -532,9 +545,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -544,25 +554,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -579,6 +577,24 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -840,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -852,52 +868,52 @@
     <col min="5" max="5" width="18.77734375" style="2" customWidth="1"/>
     <col min="6" max="6" width="61.6640625" style="2" customWidth="1"/>
     <col min="7" max="8" width="10.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="61.6640625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="61.6640625" style="8" customWidth="1"/>
     <col min="10" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-    </row>
-    <row r="2" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+    </row>
+    <row r="2" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2"/>
@@ -907,491 +923,505 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="9"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="90" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+    </row>
+    <row r="4" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="F5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:26" s="21" customFormat="1" ht="90" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="C7" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="E7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:26" s="14" customFormat="1" ht="90" customHeight="1">
-      <c r="A7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="G7" s="18"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:26" s="8" customFormat="1" ht="179.45" customHeight="1">
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:26" s="7" customFormat="1" ht="179.45" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>95</v>
+        <v>47</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="E16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>94</v>
+        <v>72</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>103</v>
+        <v>43</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
-      <c r="A24" s="2"/>
-      <c r="B24" s="1" t="s">
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1400,9 +1430,9 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1411,9 +1441,9 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1422,9 +1452,9 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1433,9 +1463,9 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" s="8" customFormat="1" ht="90" customHeight="1">
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1444,7 +1474,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="9"/>
+      <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:9" ht="90" customHeight="1"/>
     <row r="31" spans="1:9" ht="90" customHeight="1"/>
@@ -2426,9 +2456,19 @@
     <hyperlink ref="F3" r:id="rId4"/>
     <hyperlink ref="F8" display="https://fr.semrush.com/blog/balises-structurelles-html-semantique/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486542001727&amp;kwid=dsa-1100351996564&amp;cmpid=11849486850&amp;agpid=113156859297&amp;BU=Core&amp;extid=23618958962&amp;adp"/>
     <hyperlink ref="F9" display="https://fr.semrush.com/blog/balises-structurelles-html-semantique/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486542001727&amp;kwid=dsa-1100351996564&amp;cmpid=11849486850&amp;agpid=113156859297&amp;BU=Core&amp;extid=23618958962&amp;adp"/>
+    <hyperlink ref="I7" r:id="rId5" location="format"/>
+    <hyperlink ref="F14" r:id="rId6"/>
+    <hyperlink ref="F13" r:id="rId7"/>
+    <hyperlink ref="F11" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="K7" r:id="rId10"/>
+    <hyperlink ref="F19" r:id="rId11"/>
+    <hyperlink ref="F16" r:id="rId12"/>
+    <hyperlink ref="F20" r:id="rId13"/>
+    <hyperlink ref="F22" r:id="rId14" location="mf-deprecated "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup orientation="landscape" r:id="rId15"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dernier mise jour des fichier
</commit_message>
<xml_diff>
--- a/Modèle-audit.xlsx
+++ b/Modèle-audit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="630" windowWidth="23250" windowHeight="13170" tabRatio="500"/>
+    <workbookView xWindow="936" yWindow="636" windowWidth="23256" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="118">
   <si>
     <t>Catégorie</t>
   </si>
@@ -60,12 +60,6 @@
     <t xml:space="preserve">default n'est pas un langue </t>
   </si>
   <si>
-    <t>metre lang="fr" ou en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le changer </t>
-  </si>
-  <si>
     <t>https://www.w3.org/International/questions/qa-html-language-declarations.fr</t>
   </si>
   <si>
@@ -78,69 +72,36 @@
     <t xml:space="preserve">risque de bloquer le chargement de la page </t>
   </si>
   <si>
-    <t>les deplacer</t>
-  </si>
-  <si>
     <t>&lt;title&gt;.&lt;/title&gt;</t>
   </si>
   <si>
     <t>https://smartkeyword.io/seo-on-page-balise-title/#:~:text=de%20l'onglet.-,Pourquoi%20la%20balise%20Title%20est%20importante%20en%20SEO%20%3F,et%20positionner%20la%20page%20web.</t>
   </si>
   <si>
-    <t xml:space="preserve">remplacer le , par </t>
-  </si>
-  <si>
-    <t>La Panthère|Agence de web design</t>
-  </si>
-  <si>
     <t>https://www.google.com/search?q=meta+name%3D%22keywords%22&amp;rlz=1C1CHBF_frFR895FR895&amp;sxsrf=APq-WBvDYtxIkYXC0tYLkWdHGFJW8BJpkA%3A1645716124252&amp;ei=nKIXYqXMDq3BlwTXqaz4Ag&amp;ved=0ahUKEwilivKn0pj2AhWt4IUKHdcUCy8Q4dUDCA4&amp;uact=5&amp;oq=meta+name%3D%22keywords%22&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBAgjECcyBAgjECcyBQgAEIAEMgUIABDLATIGCAAQFhAeMgYIABAWEB4yBggAEBYQHjIGCAAQFhAeMgYIABAWEB4yBggAEBYQHjoHCAAQRxCwA0oECEEYAEoECEYYAFC4BFi9BmD-CGgBcAF4AIABXIgBrgGSAQEymAEAoAEByAEIwAEB&amp;sclient=gws-wiz</t>
   </si>
   <si>
     <t>meta name="keywords"</t>
   </si>
   <si>
-    <t xml:space="preserve">ne pas en utiliser car la balise  est morte voir l'article sur la mort d'une balise </t>
-  </si>
-  <si>
-    <t>n'est pas vrement utile pour le seo surtout quand spamer de la sorte</t>
-  </si>
-  <si>
     <t>code non valide w3c</t>
   </si>
   <si>
     <t>le validateur de code trouve des erreurs</t>
   </si>
   <si>
-    <t>definir une routine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toujours validée sont code avant de le push </t>
-  </si>
-  <si>
     <t>https://validator.w3.org/</t>
   </si>
   <si>
     <t>Des balise div on etais utiliser à la place des balises sementiques</t>
   </si>
   <si>
-    <t>revoir l'utilisation des balise sementique</t>
-  </si>
-  <si>
-    <t>utiliser des balise sementique</t>
-  </si>
-  <si>
     <t>https://fr.semrush.com/blog/balises-structurelles-html-semantique/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486542001727&amp;kwid=dsa-1100351996564&amp;cmpid=11849486850&amp;agpid=113156859297&amp;BU=Core&amp;extid=23618958962&amp;adpos=&amp;gclid=CjwKCAiA9tyQBhAIEiwA6tdCrDmTXE7wM4xuXZzZkjFa2YxmKn6u6fZlQAvOMotviWFd63UTxVabChoCpYcQAvD_BwE</t>
   </si>
   <si>
     <t>evtiter les declaration css dans le html</t>
   </si>
   <si>
-    <t>ne pas se servire des inline et essayer de se servire du moin possible dela balise id</t>
-  </si>
-  <si>
-    <t>donnais une classe si il ni en a pas et reporter le css dans le fichierprevu à cette effet</t>
-  </si>
-  <si>
     <t>pour l'ordre seul un !important peut prendre le dessu d'un inline</t>
   </si>
   <si>
@@ -150,9 +111,6 @@
     <t>https://www.webrankinfo.com/dossiers/debutants/meta-keywords#format</t>
   </si>
   <si>
-    <t>la remplacer par une balise descrription</t>
-  </si>
-  <si>
     <t>https://www.webrankinfo.com/dossiers/debutants/balise-title</t>
   </si>
   <si>
@@ -213,21 +171,9 @@
     <t xml:space="preserve">avoire un annuaire qualitatif plutôt que quantitatif </t>
   </si>
   <si>
-    <t xml:space="preserve">eviter le spam </t>
-  </si>
-  <si>
     <t>police &lt;12px</t>
   </si>
   <si>
-    <t xml:space="preserve">taille des police trop petite pour que cela soit que le soit sure sue cela est lisible </t>
-  </si>
-  <si>
-    <t xml:space="preserve">toujour avoir des police superieur a 12 px </t>
-  </si>
-  <si>
-    <t xml:space="preserve">augmenter la taille des polices </t>
-  </si>
-  <si>
     <t>accessiblité</t>
   </si>
   <si>
@@ -237,18 +183,12 @@
     <t xml:space="preserve">le texte en image ne peut pas etre lu avec un assistent vocal donc et invisible </t>
   </si>
   <si>
-    <t>toujours ecrire le texte en dure quand cela est possible ou remplire la balise alt _</t>
-  </si>
-  <si>
     <t>remplacer les image par des balise p</t>
   </si>
   <si>
     <t xml:space="preserve">probleme de contraste </t>
   </si>
   <si>
-    <t xml:space="preserve">changer les couleur de certaine section du site </t>
-  </si>
-  <si>
     <t xml:space="preserve">Correction du chemin du fichier .css et .js </t>
   </si>
   <si>
@@ -270,15 +210,9 @@
     <t>utiliser les bonne balise la une balise i me parais plus pertinente</t>
   </si>
   <si>
-    <t>utiliser les balise les plus coherante possible</t>
-  </si>
-  <si>
     <t>input et texte area ne sont pas dans notre label</t>
   </si>
   <si>
-    <t>ou attribuer l'attribue for a mon input et a mon texte area</t>
-  </si>
-  <si>
     <t xml:space="preserve">modification du format des image </t>
   </si>
   <si>
@@ -288,12 +222,6 @@
     <t xml:space="preserve">les images sont trop lourde </t>
   </si>
   <si>
-    <t>modifier le format des image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">convertire les image au format  WebP ou AVIF </t>
-  </si>
-  <si>
     <t>https://web.dev/color-contrast/?utm_source=lighthouse&amp;utm_medium=lr</t>
   </si>
   <si>
@@ -303,9 +231,6 @@
     <t>best practices/seo</t>
   </si>
   <si>
-    <t xml:space="preserve">ajout de escription pertinente dans les balise alt </t>
-  </si>
-  <si>
     <t xml:space="preserve">les balise alt sont mal remplie </t>
   </si>
   <si>
@@ -319,9 +244,6 @@
   </si>
   <si>
     <t>remplacer les image par les max-device-width  par des device-width</t>
-  </si>
-  <si>
-    <t>cette commande a etais deprecier</t>
   </si>
   <si>
     <r>
@@ -351,9 +273,6 @@
     <t>ne sont pas des valeur accepter pour un padding-left ou right</t>
   </si>
   <si>
-    <t>verifier toujours les valuer accepeter par nos ligne de commande</t>
-  </si>
-  <si>
     <t>les supprimer ou les remplacer pour avoir l'effet escompter</t>
   </si>
   <si>
@@ -364,9 +283,6 @@
   </si>
   <si>
     <t>https://geekflare.com/fr/remove-seo-spam/</t>
-  </si>
-  <si>
-    <t>bon sens</t>
   </si>
   <si>
     <t>https://web.dev/font-size/?utm_source=lighthouse&amp;utm_medium=lr</t>
@@ -382,9 +298,6 @@
     <t>toujour verifier le ratio entre le background et les font</t>
   </si>
   <si>
-    <t>wrapper input et le texte area dans le label</t>
-  </si>
-  <si>
     <t>suppression des li non utiliser</t>
   </si>
   <si>
@@ -397,9 +310,6 @@
     <t>balise li non utile</t>
   </si>
   <si>
-    <t>remplire la balise alt de fasson pertinente</t>
-  </si>
-  <si>
     <t>https://web.dev/label/?utm_source=lighthouse&amp;utm_medium=lr</t>
   </si>
   <si>
@@ -407,13 +317,100 @@
   </si>
   <si>
     <t xml:space="preserve">https://drafts.csswg.org/mediaqueries/#mf-deprecated </t>
+  </si>
+  <si>
+    <t>metre lang="fr" ou "en"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">definir une routine de toujours validée sont code avant de le push </t>
+  </si>
+  <si>
+    <t>corriger les erreurs toruvé par le validateur</t>
+  </si>
+  <si>
+    <t>modifier avec une langue valide</t>
+  </si>
+  <si>
+    <t>les déplacer</t>
+  </si>
+  <si>
+    <t>remplacer le , par  "La Panthère|Agence de web design"</t>
+  </si>
+  <si>
+    <t>mettre un titre pertinent car ce titre se retrouve dans la barre de titre du navigateur mais également dans les pages de résultats des moteurs de recherche </t>
+  </si>
+  <si>
+    <t>ne jamais spamer des mot clef pour tricher au niveau du seo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n'est pas vrement utile pour le seo google mais peu etre utile pour les autre si elle est corectement remplis </t>
+  </si>
+  <si>
+    <t>la remplacer sont contenue par du contenue pertinent</t>
+  </si>
+  <si>
+    <t>toujours utiliser des balise sementique</t>
+  </si>
+  <si>
+    <t>modifier le code pour integrais des balises sementiques</t>
+  </si>
+  <si>
+    <t>ne pas se servire des inline et essayer de se servire du moin possible des id</t>
+  </si>
+  <si>
+    <t>diminuer la specificité du code</t>
+  </si>
+  <si>
+    <t>supression de l'annuaire le temps d'avoir des partenaire de qualité</t>
+  </si>
+  <si>
+    <t>Toujours avoir des polices superieur à 12 px ,</t>
+  </si>
+  <si>
+    <t>Augmenter la taille des polices ,</t>
+  </si>
+  <si>
+    <t>Taille des police trop petite pour que cela soit lisible,</t>
+  </si>
+  <si>
+    <t>toujours ecrire le texte en "dure" quand cela est possible ou remplire la balise alt _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer les couleur de certaine partie du site </t>
+  </si>
+  <si>
+    <t>modification de la balise a par une balise i</t>
+  </si>
+  <si>
+    <t>wrapper input et le texte area dans le label ou leur atribue à chacun un for.</t>
+  </si>
+  <si>
+    <t>ratacher l'input et le textarea à mon label.</t>
+  </si>
+  <si>
+    <t>modifier le format des image en WebP ou AVIF</t>
+  </si>
+  <si>
+    <t>utiliser les meilleur format d'images possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajout de description pertinente dans les attribut alt </t>
+  </si>
+  <si>
+    <t>remplire les balises alt de fasson pertinente</t>
+  </si>
+  <si>
+    <t>cette commande à etais deprecier</t>
+  </si>
+  <si>
+    <t>verifier toujours les valeurs accepeter par nos ligne de commande</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -487,6 +484,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -525,7 +528,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -595,6 +598,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -856,20 +868,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="21.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="61.6640625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="10.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="61.6640625" style="8" customWidth="1"/>
-    <col min="10" max="26" width="10.5546875" customWidth="1"/>
+    <col min="1" max="2" width="21.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.90625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="61.6328125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10.54296875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="61.6328125" style="8" customWidth="1"/>
+    <col min="10" max="26" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -930,19 +942,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
@@ -956,13 +968,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
@@ -973,42 +985,42 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
+    <row r="6" spans="1:26" s="7" customFormat="1" ht="121.8" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>95</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
@@ -1019,70 +1031,70 @@
         <v>7</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>40</v>
+        <v>17</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>98</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="20"/>
       <c r="I7" s="22" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:26" s="7" customFormat="1" ht="179.45" customHeight="1">
+    <row r="9" spans="1:26" s="7" customFormat="1" ht="179.4" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1093,19 +1105,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1116,19 +1128,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1136,23 +1148,21 @@
     </row>
     <row r="12" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="8"/>
@@ -1162,19 +1172,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>60</v>
+        <v>45</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1182,22 +1192,22 @@
     </row>
     <row r="14" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1205,19 +1215,19 @@
     </row>
     <row r="15" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1226,22 +1236,22 @@
     </row>
     <row r="16" spans="1:26" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="F16" s="6" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1252,16 +1262,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1273,16 +1283,16 @@
         <v>7</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1294,42 +1304,42 @@
         <v>7</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="F19" s="6" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="8"/>
+      <c r="I19" s="26"/>
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1337,16 +1347,16 @@
     </row>
     <row r="21" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>115</v>
@@ -1358,22 +1368,22 @@
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1381,19 +1391,19 @@
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1402,19 +1412,19 @@
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" ht="90" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1425,7 +1435,6 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>

</xml_diff>